<commit_message>
Fixed Issue with 3.3v regulator overpowering
</commit_message>
<xml_diff>
--- a/Arduino_Nano/BOM_Arduino_Nano.xlsx
+++ b/Arduino_Nano/BOM_Arduino_Nano.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df288a9f25243d92/Research/4-D-Avionic-Systems/EC191_Cirr/AutonoMouse/Arduino_Nano/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_A4743FB22242ABB19E13D11929075D3FDE875012" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF51FFF8-341C-4D95-9568-9CBD096E9E4F}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_A4743FB22242ABB19E13D11929075D3FDE875012" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270B089C-6E91-47CA-89A5-A611F0EA188A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="10170" yWindow="2580" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonoMouse" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Arduino Nano wout/RC</t>
   </si>
@@ -78,12 +78,6 @@
     <t>Female Header Pins</t>
   </si>
   <si>
-    <t>Sonar Sensor</t>
-  </si>
-  <si>
-    <t>Power Indicator LED</t>
-  </si>
-  <si>
     <t>Acrylic</t>
   </si>
   <si>
@@ -108,10 +102,19 @@
     <t>$0.08 per in^2</t>
   </si>
   <si>
-    <t>1 inch bottle cap</t>
-  </si>
-  <si>
     <t>$0.40 per in^2</t>
+  </si>
+  <si>
+    <t>1 inch diameter bottle cap</t>
+  </si>
+  <si>
+    <t>LED Colored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Sonar </t>
+  </si>
+  <si>
+    <t>Sensor-Ultrasonic used for angry engineers</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -435,7 +438,7 @@
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -443,7 +446,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -457,9 +460,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -470,10 +473,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -488,7 +491,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -504,7 +507,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -519,7 +522,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -534,7 +537,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -549,7 +552,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -564,7 +567,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -579,7 +582,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -594,7 +597,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -609,7 +612,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -624,9 +627,9 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -639,9 +642,9 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -654,12 +657,12 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="E15" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -671,10 +674,13 @@
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -689,7 +695,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -705,7 +711,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -718,12 +724,12 @@
         <v>1.62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4">
         <v>2</v>
@@ -740,7 +746,7 @@
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="8">
         <f>SUM(D3:D20)</f>

</xml_diff>

<commit_message>
PCB and base changes
</commit_message>
<xml_diff>
--- a/Arduino_Nano/BOM_Arduino_Nano.xlsx
+++ b/Arduino_Nano/BOM_Arduino_Nano.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df288a9f25243d92/Research/4-D-Avionic-Systems/EC191_Cirr/AutonoMouse/Arduino_Nano/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_A4743FB22242ABB19E13D11929075D3FDE875012" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{270B089C-6E91-47CA-89A5-A611F0EA188A}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_A4743FB22242ABB19E13D11929075D3FDE875012" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06A424DC-D089-426E-A46F-0A1B19973312}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="10170" yWindow="2580" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonoMouse" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Arduino Nano wout/RC</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Battery Cap</t>
   </si>
   <si>
-    <t>Male header Pins</t>
-  </si>
-  <si>
-    <t>Female Header Pins</t>
-  </si>
-  <si>
     <t>Acrylic</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Continuous Servo</t>
   </si>
   <si>
-    <t>Gatorade bottles work best</t>
-  </si>
-  <si>
     <t xml:space="preserve">CABLE-USB A-Mini </t>
   </si>
   <si>
@@ -115,6 +106,24 @@
   </si>
   <si>
     <t>Sensor-Ultrasonic used for angry engineers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x15 Female header </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x4 Female header </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x3 Male header </t>
+  </si>
+  <si>
+    <t>Buy your own, Gatorade bottles work best</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>You might need to buy a larger one and then break off the pins you need</t>
   </si>
 </sst>
 </file>
@@ -189,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -205,6 +214,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,10 +437,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="A1:E21"/>
+      <selection activeCell="E22" sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -438,15 +448,15 @@
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -459,24 +469,27 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D19" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D20" si="0">B3*C3</f>
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -491,7 +504,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -507,7 +520,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -522,7 +535,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -537,7 +550,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -552,7 +565,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -567,7 +580,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -582,7 +595,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -597,160 +610,178 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C13" s="3">
-        <v>0.02</v>
+        <v>0.08</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
         <v>1.8</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <v>0.4</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F16" t="s">
-        <v>27</v>
+      <c r="E16" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>0.05</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="3">
-        <v>0.99</v>
+        <v>0.05</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>0.05</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.62</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.62</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="D21" s="6">
+        <f>B21*C21</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.62</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>1.62</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="4">
-        <v>2</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="D20" s="6">
-        <f>B20*C20</f>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="8">
-        <f>SUM(D3:D20)</f>
-        <v>19.11</v>
+      <c r="D22" s="8">
+        <f>SUM(D3:D21)</f>
+        <v>18.189999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added resistor to BOM
</commit_message>
<xml_diff>
--- a/Arduino_Nano/BOM_Arduino_Nano.xlsx
+++ b/Arduino_Nano/BOM_Arduino_Nano.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df288a9f25243d92/Research/4-D-Avionic-Systems/EC191_Cirr/AutonoMouse/Arduino_Nano/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\racha\BYU\Immerse\AutonoMouse\Arduino_Nano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="11_A4743FB22242ABB19E13D11929075D3FDE875012" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06A424DC-D089-426E-A46F-0A1B19973312}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45AA6ED-9D68-4B95-BCEF-AD7B0D45DB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2710" yWindow="0" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutonoMouse" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Arduino Nano wout/RC</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>You might need to buy a larger one and then break off the pins you need</t>
+  </si>
+  <si>
+    <t>330 Ohm Resistor</t>
   </si>
 </sst>
 </file>
@@ -198,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -214,6 +217,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,26 +441,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="A1:E22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -473,7 +477,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
@@ -482,14 +486,14 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D20" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D21" si="0">B3*C3</f>
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -503,8 +507,9 @@
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,7 +525,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -535,7 +540,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -550,7 +555,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -565,7 +570,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -580,208 +585,224 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
         <v>1.25</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
         <v>0.44</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>0.06</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
         <v>0.08</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:6" s="11" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
         <v>1.8</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C17" s="3">
         <v>0.4</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
         <v>0.05</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
         <v>0.99</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
         <v>1.62</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>1.62</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B22" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>0.06</v>
       </c>
-      <c r="D21" s="6">
-        <f>B21*C21</f>
+      <c r="D22" s="6">
+        <f>B22*C22</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="s">
+    <row r="23" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="8">
-        <f>SUM(D3:D21)</f>
-        <v>18.189999999999998</v>
+      <c r="D23" s="8">
+        <f>SUM(D3:D22)</f>
+        <v>18.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>